<commit_message>
Added successful creation message.
</commit_message>
<xml_diff>
--- a/scholarships/scholarships.xlsx
+++ b/scholarships/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,6 +497,37 @@
         <v>3.25</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cool Kids Scholarship</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>10000000</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>36</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="G3" t="n">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Edit functionality with xlsx file working
</commit_message>
<xml_diff>
--- a/scholarships/scholarships.xlsx
+++ b/scholarships/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,35 +476,56 @@
           <t>Test One</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>8000</t>
-        </is>
+      <c r="B2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="C2" t="n">
+        <v>8000</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>All</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>26</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>4.0</t>
-        </is>
+      <c r="E2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Computer Science and Engineering</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>36</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="G3" t="n">
+        <v>4.95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deletion functionality working - cleanup needed.
</commit_message>
<xml_diff>
--- a/scholarships/scholarships.xlsx
+++ b/scholarships/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,59 +473,28 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Test One</t>
+          <t>t13</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1000</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>8000</v>
+        <v>3</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>All</t>
+          <t>Computer Science and Engineering</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Cool Kids Club</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>11111111</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Computer Science and Engineering</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>36</v>
-      </c>
-      <c r="F3" t="n">
-        <v>1600</v>
-      </c>
-      <c r="G3" t="n">
-        <v>4.95</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated values in Create + example data
</commit_message>
<xml_diff>
--- a/scholarships/scholarships.xlsx
+++ b/scholarships/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -461,10 +461,20 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>SAT</t>
+          <t>SAT Math</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>SAT Reading</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>SAT Combined</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
@@ -473,28 +483,71 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>t13</t>
+          <t>Test One</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2</v>
+        <v>1000</v>
       </c>
       <c r="C2" t="n">
-        <v>3</v>
+        <v>8000</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>26</v>
+      </c>
+      <c r="F2" t="n">
+        <v>600</v>
+      </c>
+      <c r="G2" t="n">
+        <v>400</v>
+      </c>
+      <c r="H2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Cool Kids Club</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>11111111</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Computer Science and Engineering</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
+      <c r="E3" t="n">
+        <v>36</v>
+      </c>
+      <c r="F3" t="n">
+        <v>800</v>
+      </c>
+      <c r="G3" t="n">
+        <v>800</v>
+      </c>
+      <c r="H3" t="n">
+        <v>1600</v>
+      </c>
+      <c r="I3" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added in hs percentile to criteria.
</commit_message>
<xml_diff>
--- a/scholarships/scholarships.xlsx
+++ b/scholarships/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>GPA</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>HS Percentile</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -512,11 +517,14 @@
       <c r="I2" t="n">
         <v>4</v>
       </c>
+      <c r="J2" t="n">
+        <v>96</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Cool Kids Club</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -526,7 +534,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11111111</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -535,19 +543,22 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>800</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>790</v>
+        <v>0</v>
       </c>
       <c r="H3" t="n">
-        <v>1600</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="J3" t="n">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Extra inputs to the create and edit.
</commit_message>
<xml_diff>
--- a/scholarships/scholarships.xlsx
+++ b/scholarships/scholarships.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,35 +451,55 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>RAI</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Admit Score</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>Major</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>ACT</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>ACT Math</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>ACT English</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ACT Composite</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>SAT Math</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>SAT Reading</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>SAT Combined</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>GPA</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>HS Percentile</t>
         </is>
@@ -497,68 +517,92 @@
       <c r="C2" t="n">
         <v>8000</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>All</t>
-        </is>
+      <c r="D2" t="n">
+        <v>315</v>
       </c>
       <c r="E2" t="n">
         <v>26</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
+      </c>
+      <c r="G2" t="n">
+        <v>25</v>
+      </c>
+      <c r="H2" t="n">
+        <v>27</v>
+      </c>
+      <c r="I2" t="n">
+        <v>26</v>
+      </c>
+      <c r="J2" t="n">
         <v>600</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
         <v>400</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L2" t="n">
         <v>1000</v>
       </c>
-      <c r="I2" t="n">
+      <c r="M2" t="n">
         <v>4</v>
       </c>
-      <c r="J2" t="n">
+      <c r="N2" t="n">
         <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>Test Two</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>50</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Computer Science and Engineering</t>
-        </is>
+          <t>10000</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>330</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>All</t>
+        </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="H3" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="I3" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J3" t="n">
-        <v>31</v>
+        <v>700</v>
+      </c>
+      <c r="K3" t="n">
+        <v>620</v>
+      </c>
+      <c r="L3" t="n">
+        <v>1320</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3.8</v>
+      </c>
+      <c r="N3" t="n">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>